<commit_message>
Updated final dataset and finalized figures.
</commit_message>
<xml_diff>
--- a/DataRe-Analysis/SummaryAnalysis_Dataset_v7.xlsx
+++ b/DataRe-Analysis/SummaryAnalysis_Dataset_v7.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25725"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="140" yWindow="0" windowWidth="28180" windowHeight="15800" tabRatio="867" activeTab="5"/>
+    <workbookView xWindow="3580" yWindow="0" windowWidth="24840" windowHeight="15720" tabRatio="954"/>
   </bookViews>
   <sheets>
     <sheet name="Antibodies-PRE" sheetId="15" r:id="rId1"/>
@@ -13,9 +13,10 @@
     <sheet name="Organisms- POST" sheetId="5" r:id="rId4"/>
     <sheet name="Software-PRE" sheetId="10" r:id="rId5"/>
     <sheet name="Software- POST C v NC" sheetId="18" r:id="rId6"/>
-    <sheet name="Figure" sheetId="19" r:id="rId7"/>
-    <sheet name="Fig3 Analysis" sheetId="16" r:id="rId8"/>
+    <sheet name="Figure 3" sheetId="19" r:id="rId7"/>
+    <sheet name="Figure 4" sheetId="16" r:id="rId8"/>
     <sheet name="binary significance test" sheetId="17" r:id="rId9"/>
+    <sheet name="Correct usage" sheetId="20" r:id="rId10"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7820" uniqueCount="1499">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7697" uniqueCount="1504">
   <si>
     <t>Organisms</t>
   </si>
@@ -4847,15 +4848,31 @@
   <si>
     <t>Analysis for all resources: Predictive value</t>
   </si>
+  <si>
+    <t>Number incorrect</t>
+  </si>
+  <si>
+    <t>Total number</t>
+  </si>
+  <si>
+    <t>Correct usage (number incorrect)</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Error rate</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="74" x14ac:knownFonts="1">
+  <fonts count="75" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -5217,6 +5234,10 @@
       <color theme="10"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Times New Roman"/>
+    </font>
   </fonts>
   <fills count="16">
     <fill>
@@ -5429,7 +5450,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="752">
+  <cellStyleXfs count="780">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="2" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="39" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -6182,8 +6203,36 @@
     <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="73" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="73" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="73" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="73" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="73" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="73" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="73" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="73" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="73" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="73" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="73" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="73" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="73" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="73" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="73" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="269">
+  <cellXfs count="275">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -6736,21 +6785,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="47" fillId="5" borderId="1" xfId="150" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="46" fillId="9" borderId="1" xfId="150" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="59" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -6775,8 +6809,35 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="28" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="5" borderId="1" xfId="150" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="9" borderId="1" xfId="150" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="159" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="159" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="74" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="51" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="752">
+  <cellStyles count="780">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
@@ -7514,6 +7575,20 @@
     <cellStyle name="Followed Hyperlink" xfId="747" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="749" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="751" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="753" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="755" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="757" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="759" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="761" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="763" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="765" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="767" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="769" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="771" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="773" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="775" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="777" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="779" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="732" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="734" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="736" builtinId="8" hidden="1"/>
@@ -7524,6 +7599,20 @@
     <cellStyle name="Hyperlink" xfId="746" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="748" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="750" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="752" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="754" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="756" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="758" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="760" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="762" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="764" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="766" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="768" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="770" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="772" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="774" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="776" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="778" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="3"/>
     <cellStyle name="Normal 3" xfId="150"/>
@@ -7561,7 +7650,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Figure!$B$25</c:f>
+              <c:f>'Figure 3'!$B$25</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -7578,7 +7667,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Figure!$B$26:$B$28</c:f>
+              <c:f>'Figure 3'!$B$26:$B$28</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="3"/>
@@ -7589,7 +7678,7 @@
                   <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.918141592920354</c:v>
+                  <c:v>0.911057692307692</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7600,7 +7689,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Figure!$C$25</c:f>
+              <c:f>'Figure 3'!$C$25</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -7617,7 +7706,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Figure!$C$26:$C$28</c:f>
+              <c:f>'Figure 3'!$C$26:$C$28</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="3"/>
@@ -7628,7 +7717,7 @@
                   <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.933333333333333</c:v>
+                  <c:v>0.846153846153846</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7639,7 +7728,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Figure!$D$25</c:f>
+              <c:f>'Figure 3'!$D$25</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -7656,18 +7745,18 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Figure!$D$26:$D$28</c:f>
+              <c:f>'Figure 3'!$D$26:$D$28</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0.802083333333333</c:v>
+                  <c:v>0.791666666666667</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.9625</c:v>
+                  <c:v>0.962025316455696</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.98989898989899</c:v>
+                  <c:v>0.987179487179487</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7682,11 +7771,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2103279032"/>
-        <c:axId val="2103282136"/>
+        <c:axId val="-2114916872"/>
+        <c:axId val="-2114920040"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2103279032"/>
+        <c:axId val="-2114916872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7709,7 +7798,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2103282136"/>
+        <c:crossAx val="-2114920040"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7717,7 +7806,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2103282136"/>
+        <c:axId val="-2114920040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -7741,7 +7830,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2103279032"/>
+        <c:crossAx val="-2114916872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.2"/>
@@ -7822,7 +7911,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Fig3 Analysis'!$A$3</c:f>
+              <c:f>'Figure 4'!$A$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -7845,7 +7934,7 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>'Fig3 Analysis'!$C$29:$C$31</c:f>
+                <c:f>'Figure 4'!$C$29:$C$31</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
@@ -7863,7 +7952,7 @@
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>'Fig3 Analysis'!$B$29:$B$31</c:f>
+                <c:f>'Figure 4'!$B$29:$B$31</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
@@ -7882,7 +7971,7 @@
           </c:errBars>
           <c:val>
             <c:numRef>
-              <c:f>'Fig3 Analysis'!$B$3:$D$3</c:f>
+              <c:f>'Figure 4'!$B$3:$D$3</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="3"/>
@@ -7904,7 +7993,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Fig3 Analysis'!$A$4</c:f>
+              <c:f>'Figure 4'!$A$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -7928,12 +8017,12 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>'Fig3 Analysis'!$F$29:$F$31</c:f>
+                <c:f>'Figure 4'!$F$29:$F$31</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
                   <c:pt idx="0">
-                    <c:v>0.0166344036697248</c:v>
+                    <c:v>0.0160530088495575</c:v>
                   </c:pt>
                   <c:pt idx="1">
                     <c:v>0.0616151851851853</c:v>
@@ -7946,12 +8035,12 @@
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>'Fig3 Analysis'!$E$29:$E$31</c:f>
+                <c:f>'Figure 4'!$E$29:$E$31</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
                   <c:pt idx="0">
-                    <c:v>0.0231755963302752</c:v>
+                    <c:v>0.0223869911504425</c:v>
                   </c:pt>
                   <c:pt idx="1">
                     <c:v>0.0759248148148147</c:v>
@@ -7965,12 +8054,12 @@
           </c:errBars>
           <c:val>
             <c:numRef>
-              <c:f>'Fig3 Analysis'!$B$4:$D$4</c:f>
+              <c:f>'Figure 4'!$B$4:$D$4</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0.958715596330275</c:v>
+                  <c:v>0.960176991150442</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.814814814814815</c:v>
@@ -7991,11 +8080,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2117165400"/>
-        <c:axId val="-2117162312"/>
+        <c:axId val="-2093623272"/>
+        <c:axId val="-2093620184"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2117165400"/>
+        <c:axId val="-2093623272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8018,7 +8107,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2117162312"/>
+        <c:crossAx val="-2093620184"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8026,7 +8115,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2117162312"/>
+        <c:axId val="-2093620184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -8050,7 +8139,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2117165400"/>
+        <c:crossAx val="-2093623272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.2"/>
@@ -8487,9 +8576,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R144"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H112" sqref="H112"/>
+      <selection pane="bottomLeft" activeCell="P4" sqref="P4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -14088,13 +14177,115 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="14.33203125" style="13" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="36">
+      <c r="B1" s="13" t="s">
+        <v>1501</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1502</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1503</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="13">
+        <f>'Antibody-POST 1st vs 2nd Abs'!F458</f>
+        <v>37</v>
+      </c>
+      <c r="C2">
+        <f>'Antibody-POST 1st vs 2nd Abs'!F459</f>
+        <v>416</v>
+      </c>
+      <c r="D2" s="156">
+        <f>B2/C2</f>
+        <v>8.8942307692307696E-2</v>
+      </c>
+      <c r="E2" s="156"/>
+      <c r="G2" s="272"/>
+      <c r="H2" s="273"/>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="13">
+        <f>'Organisms- POST'!F141</f>
+        <v>8</v>
+      </c>
+      <c r="C3">
+        <f>'Organisms- POST'!F142</f>
+        <v>52</v>
+      </c>
+      <c r="D3" s="156">
+        <f>B3/C3</f>
+        <v>0.15384615384615385</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="13">
+        <f>'Software- POST C v NC'!F104</f>
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <f>'Software- POST C v NC'!F105</f>
+        <v>78</v>
+      </c>
+      <c r="D4" s="156">
+        <f t="shared" ref="D3:D4" si="0">B4/C4</f>
+        <v>1.282051282051282E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" t="s">
+        <v>1502</v>
+      </c>
+      <c r="B6" s="13">
+        <f>SUM(B2:B4)</f>
+        <v>46</v>
+      </c>
+      <c r="C6">
+        <f>SUM(C2:C4)</f>
+        <v>546</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V472"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B1" sqref="B1:B1048576"/>
+      <selection pane="bottomLeft" activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -14184,12 +14375,12 @@
         <v>1374</v>
       </c>
       <c r="J2" s="112">
-        <f>COUNTIF(G4:G439,"y")</f>
-        <v>418</v>
+        <f>COUNTIF(G4:G455,"y")</f>
+        <v>434</v>
       </c>
       <c r="K2" s="112">
-        <f>COUNTA(G4:G439)</f>
-        <v>436</v>
+        <f>COUNTA(G4:G455)</f>
+        <v>452</v>
       </c>
       <c r="L2" s="55"/>
       <c r="M2" s="55"/>
@@ -14207,7 +14398,7 @@
       <c r="A3" s="124"/>
       <c r="B3" s="143"/>
       <c r="C3" s="144"/>
-      <c r="D3" s="267">
+      <c r="D3" s="262">
         <f>COUNTIF(D4:D455,"y")</f>
         <v>416</v>
       </c>
@@ -14217,7 +14408,7 @@
       </c>
       <c r="F3" s="211">
         <f>COUNTIF(F4:F455,"y")</f>
-        <v>415</v>
+        <v>379</v>
       </c>
       <c r="G3" s="185"/>
       <c r="H3" s="145"/>
@@ -14250,9 +14441,7 @@
       <c r="E4" s="165" t="s">
         <v>1415</v>
       </c>
-      <c r="F4" s="165" t="s">
-        <v>3</v>
-      </c>
+      <c r="F4" s="165"/>
       <c r="G4" s="62" t="s">
         <v>3</v>
       </c>
@@ -14279,9 +14468,7 @@
       <c r="E5" s="165" t="s">
         <v>1415</v>
       </c>
-      <c r="F5" s="165" t="s">
-        <v>3</v>
-      </c>
+      <c r="F5" s="165"/>
       <c r="G5" s="62" t="s">
         <v>3</v>
       </c>
@@ -14308,9 +14495,7 @@
       <c r="E6" s="165" t="s">
         <v>1415</v>
       </c>
-      <c r="F6" s="165" t="s">
-        <v>3</v>
-      </c>
+      <c r="F6" s="165"/>
       <c r="G6" s="62" t="s">
         <v>3</v>
       </c>
@@ -14335,9 +14520,7 @@
       <c r="E7" s="165" t="s">
         <v>1415</v>
       </c>
-      <c r="F7" s="165" t="s">
-        <v>3</v>
-      </c>
+      <c r="F7" s="165"/>
       <c r="G7" s="62" t="s">
         <v>3</v>
       </c>
@@ -14362,9 +14545,7 @@
       <c r="E8" s="165" t="s">
         <v>1415</v>
       </c>
-      <c r="F8" s="165" t="s">
-        <v>3</v>
-      </c>
+      <c r="F8" s="165"/>
       <c r="G8" s="62" t="s">
         <v>3</v>
       </c>
@@ -14389,9 +14570,7 @@
       <c r="E9" s="165" t="s">
         <v>1415</v>
       </c>
-      <c r="F9" s="165" t="s">
-        <v>3</v>
-      </c>
+      <c r="F9" s="165"/>
       <c r="G9" s="62" t="s">
         <v>3</v>
       </c>
@@ -14418,9 +14597,7 @@
       <c r="E10" s="165" t="s">
         <v>1415</v>
       </c>
-      <c r="F10" s="165" t="s">
-        <v>3</v>
-      </c>
+      <c r="F10" s="165"/>
       <c r="G10" s="62" t="s">
         <v>3</v>
       </c>
@@ -14445,9 +14622,7 @@
       <c r="E11" s="165" t="s">
         <v>1415</v>
       </c>
-      <c r="F11" s="165" t="s">
-        <v>3</v>
-      </c>
+      <c r="F11" s="165"/>
       <c r="G11" s="62" t="s">
         <v>7</v>
       </c>
@@ -14474,9 +14649,7 @@
       <c r="E12" s="165" t="s">
         <v>1415</v>
       </c>
-      <c r="F12" s="165" t="s">
-        <v>3</v>
-      </c>
+      <c r="F12" s="165"/>
       <c r="G12" s="62" t="s">
         <v>7</v>
       </c>
@@ -14501,9 +14674,7 @@
       <c r="E13" s="165" t="s">
         <v>1415</v>
       </c>
-      <c r="F13" s="165" t="s">
-        <v>3</v>
-      </c>
+      <c r="F13" s="165"/>
       <c r="G13" s="62" t="s">
         <v>3</v>
       </c>
@@ -14530,9 +14701,7 @@
       <c r="E14" s="182" t="s">
         <v>1415</v>
       </c>
-      <c r="F14" s="165" t="s">
-        <v>3</v>
-      </c>
+      <c r="F14" s="165"/>
       <c r="G14" s="186" t="s">
         <v>7</v>
       </c>
@@ -14559,9 +14728,7 @@
       <c r="E15" s="165" t="s">
         <v>1415</v>
       </c>
-      <c r="F15" s="165" t="s">
-        <v>3</v>
-      </c>
+      <c r="F15" s="165"/>
       <c r="G15" s="62" t="s">
         <v>7</v>
       </c>
@@ -14588,9 +14755,7 @@
       <c r="E16" s="165" t="s">
         <v>1415</v>
       </c>
-      <c r="F16" s="165" t="s">
-        <v>3</v>
-      </c>
+      <c r="F16" s="165"/>
       <c r="G16" s="62" t="s">
         <v>7</v>
       </c>
@@ -14617,9 +14782,7 @@
       <c r="E17" s="165" t="s">
         <v>1415</v>
       </c>
-      <c r="F17" s="165" t="s">
-        <v>3</v>
-      </c>
+      <c r="F17" s="165"/>
       <c r="G17" s="62" t="s">
         <v>7</v>
       </c>
@@ -14646,9 +14809,7 @@
       <c r="E18" s="165" t="s">
         <v>1415</v>
       </c>
-      <c r="F18" s="165" t="s">
-        <v>3</v>
-      </c>
+      <c r="F18" s="165"/>
       <c r="G18" s="62" t="s">
         <v>7</v>
       </c>
@@ -14673,9 +14834,7 @@
       <c r="E19" s="165" t="s">
         <v>1415</v>
       </c>
-      <c r="F19" s="165" t="s">
-        <v>3</v>
-      </c>
+      <c r="F19" s="165"/>
       <c r="G19" s="62" t="s">
         <v>3</v>
       </c>
@@ -14700,9 +14859,7 @@
       <c r="E20" s="165" t="s">
         <v>1415</v>
       </c>
-      <c r="F20" s="165" t="s">
-        <v>3</v>
-      </c>
+      <c r="F20" s="165"/>
       <c r="G20" s="62" t="s">
         <v>3</v>
       </c>
@@ -14729,9 +14886,7 @@
       <c r="E21" s="165" t="s">
         <v>1415</v>
       </c>
-      <c r="F21" s="165" t="s">
-        <v>3</v>
-      </c>
+      <c r="F21" s="165"/>
       <c r="G21" s="62" t="s">
         <v>3</v>
       </c>
@@ -14758,9 +14913,7 @@
       <c r="E22" s="165" t="s">
         <v>1415</v>
       </c>
-      <c r="F22" s="165" t="s">
-        <v>3</v>
-      </c>
+      <c r="F22" s="165"/>
       <c r="G22" s="62" t="s">
         <v>3</v>
       </c>
@@ -14787,9 +14940,7 @@
       <c r="E23" s="165" t="s">
         <v>1415</v>
       </c>
-      <c r="F23" s="165" t="s">
-        <v>3</v>
-      </c>
+      <c r="F23" s="165"/>
       <c r="G23" s="62" t="s">
         <v>3</v>
       </c>
@@ -14814,9 +14965,7 @@
       <c r="E24" s="165" t="s">
         <v>1415</v>
       </c>
-      <c r="F24" s="165" t="s">
-        <v>3</v>
-      </c>
+      <c r="F24" s="165"/>
       <c r="G24" s="62" t="s">
         <v>3</v>
       </c>
@@ -14843,9 +14992,7 @@
       <c r="E25" s="165" t="s">
         <v>1415</v>
       </c>
-      <c r="F25" s="165" t="s">
-        <v>3</v>
-      </c>
+      <c r="F25" s="165"/>
       <c r="G25" s="62" t="s">
         <v>3</v>
       </c>
@@ -14870,9 +15017,7 @@
       <c r="E26" s="165" t="s">
         <v>1415</v>
       </c>
-      <c r="F26" s="165" t="s">
-        <v>3</v>
-      </c>
+      <c r="F26" s="165"/>
       <c r="G26" s="62" t="s">
         <v>7</v>
       </c>
@@ -14897,9 +15042,7 @@
       <c r="E27" s="165" t="s">
         <v>1415</v>
       </c>
-      <c r="F27" s="165" t="s">
-        <v>3</v>
-      </c>
+      <c r="F27" s="165"/>
       <c r="G27" s="62" t="s">
         <v>7</v>
       </c>
@@ -14924,9 +15067,7 @@
       <c r="E28" s="182" t="s">
         <v>1415</v>
       </c>
-      <c r="F28" s="165" t="s">
-        <v>3</v>
-      </c>
+      <c r="F28" s="165"/>
       <c r="G28" s="63" t="s">
         <v>7</v>
       </c>
@@ -14964,9 +15105,7 @@
       <c r="E29" s="182" t="s">
         <v>1415</v>
       </c>
-      <c r="F29" s="165" t="s">
-        <v>3</v>
-      </c>
+      <c r="F29" s="165"/>
       <c r="G29" s="63" t="s">
         <v>7</v>
       </c>
@@ -14991,9 +15130,7 @@
       <c r="E30" s="182" t="s">
         <v>1415</v>
       </c>
-      <c r="F30" s="165" t="s">
-        <v>3</v>
-      </c>
+      <c r="F30" s="165"/>
       <c r="G30" s="186" t="s">
         <v>3</v>
       </c>
@@ -15018,9 +15155,7 @@
       <c r="E31" s="165" t="s">
         <v>1415</v>
       </c>
-      <c r="F31" s="165" t="s">
-        <v>3</v>
-      </c>
+      <c r="F31" s="165"/>
       <c r="G31" s="62" t="s">
         <v>7</v>
       </c>
@@ -15045,9 +15180,7 @@
       <c r="E32" s="165" t="s">
         <v>1415</v>
       </c>
-      <c r="F32" s="165" t="s">
-        <v>3</v>
-      </c>
+      <c r="F32" s="165"/>
       <c r="G32" s="62" t="s">
         <v>7</v>
       </c>
@@ -15072,9 +15205,7 @@
       <c r="E33" s="165" t="s">
         <v>1415</v>
       </c>
-      <c r="F33" s="165" t="s">
-        <v>3</v>
-      </c>
+      <c r="F33" s="165"/>
       <c r="G33" s="62" t="s">
         <v>7</v>
       </c>
@@ -15099,9 +15230,7 @@
       <c r="E34" s="159" t="s">
         <v>1415</v>
       </c>
-      <c r="F34" s="165" t="s">
-        <v>3</v>
-      </c>
+      <c r="F34" s="165"/>
       <c r="G34" s="193" t="s">
         <v>3</v>
       </c>
@@ -15126,9 +15255,7 @@
       <c r="E35" s="159" t="s">
         <v>1415</v>
       </c>
-      <c r="F35" s="165" t="s">
-        <v>3</v>
-      </c>
+      <c r="F35" s="165"/>
       <c r="G35" s="193" t="s">
         <v>3</v>
       </c>
@@ -15153,9 +15280,7 @@
       <c r="E36" s="165" t="s">
         <v>1415</v>
       </c>
-      <c r="F36" s="165" t="s">
-        <v>3</v>
-      </c>
+      <c r="F36" s="165"/>
       <c r="G36" s="62" t="s">
         <v>7</v>
       </c>
@@ -15182,9 +15307,7 @@
       <c r="E37" s="165" t="s">
         <v>1415</v>
       </c>
-      <c r="F37" s="165" t="s">
-        <v>3</v>
-      </c>
+      <c r="F37" s="165"/>
       <c r="G37" s="62" t="s">
         <v>7</v>
       </c>
@@ -15211,9 +15334,7 @@
       <c r="E38" s="165" t="s">
         <v>1415</v>
       </c>
-      <c r="F38" s="165" t="s">
-        <v>3</v>
-      </c>
+      <c r="F38" s="165"/>
       <c r="G38" s="62" t="s">
         <v>7</v>
       </c>
@@ -15238,9 +15359,7 @@
       <c r="E39" s="165" t="s">
         <v>1415</v>
       </c>
-      <c r="F39" s="165" t="s">
-        <v>3</v>
-      </c>
+      <c r="F39" s="165"/>
       <c r="G39" s="62" t="s">
         <v>3</v>
       </c>
@@ -27296,7 +27415,9 @@
     <row r="457" spans="1:9">
       <c r="D457" s="56"/>
       <c r="E457" s="57"/>
-      <c r="F457" s="57"/>
+      <c r="F457" s="269" t="s">
+        <v>1493</v>
+      </c>
       <c r="G457" s="56"/>
       <c r="H457" s="52"/>
       <c r="I457" s="58"/>
@@ -27309,8 +27430,13 @@
         <f>COUNTIF(D40:D455,"y")</f>
         <v>416</v>
       </c>
-      <c r="E458" s="164"/>
-      <c r="F458" s="164"/>
+      <c r="E458" s="164" t="s">
+        <v>1499</v>
+      </c>
+      <c r="F458" s="164">
+        <f>COUNTIF(F4:F456,"n")</f>
+        <v>37</v>
+      </c>
       <c r="G458" s="56"/>
       <c r="H458" s="52"/>
       <c r="I458" s="58"/>
@@ -27324,6 +27450,13 @@
         <f>COUNTIF(E40:E455,"TP")</f>
         <v>416</v>
       </c>
+      <c r="E459" s="168" t="s">
+        <v>1500</v>
+      </c>
+      <c r="F459" s="168">
+        <f>COUNTA(F4:F455)</f>
+        <v>416</v>
+      </c>
       <c r="H459" s="57"/>
       <c r="I459" s="57"/>
     </row>
@@ -27336,6 +27469,7 @@
         <f>COUNTIF(E40:E455,"TN")</f>
         <v>0</v>
       </c>
+      <c r="F460" s="274"/>
       <c r="H460" s="57"/>
       <c r="I460" s="57"/>
     </row>
@@ -27454,7 +27588,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O3" sqref="O3:O60"/>
+      <selection pane="bottomLeft" activeCell="P3" sqref="P3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -29450,9 +29584,9 @@
   <dimension ref="A1:I1010"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="4" topLeftCell="A79" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="B1" sqref="B1:B1048576"/>
+      <selection pane="bottomLeft" activeCell="F119" sqref="F119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -29538,14 +29672,14 @@
       <c r="A4" s="124"/>
       <c r="B4" s="204"/>
       <c r="C4" s="205"/>
-      <c r="D4" s="268">
+      <c r="D4" s="263">
         <f>COUNTIF(D5:D139,"y")</f>
         <v>52</v>
       </c>
       <c r="E4" s="206"/>
       <c r="F4" s="211">
         <f>COUNTIF(F5:F456,"y")</f>
-        <v>126</v>
+        <v>44</v>
       </c>
       <c r="G4" s="127"/>
       <c r="H4" s="10"/>
@@ -29567,9 +29701,7 @@
       <c r="E5" s="130" t="s">
         <v>1415</v>
       </c>
-      <c r="F5" s="130" t="s">
-        <v>3</v>
-      </c>
+      <c r="F5" s="130"/>
       <c r="G5" s="15" t="s">
         <v>196</v>
       </c>
@@ -29592,9 +29724,7 @@
       <c r="E6" s="130" t="s">
         <v>1415</v>
       </c>
-      <c r="F6" s="130" t="s">
-        <v>3</v>
-      </c>
+      <c r="F6" s="130"/>
       <c r="G6" s="15" t="s">
         <v>522</v>
       </c>
@@ -29617,9 +29747,7 @@
       <c r="E7" s="130" t="s">
         <v>1415</v>
       </c>
-      <c r="F7" s="130" t="s">
-        <v>3</v>
-      </c>
+      <c r="F7" s="130"/>
       <c r="G7" s="15" t="s">
         <v>529</v>
       </c>
@@ -29642,9 +29770,7 @@
       <c r="E8" s="130" t="s">
         <v>1415</v>
       </c>
-      <c r="F8" s="130" t="s">
-        <v>3</v>
-      </c>
+      <c r="F8" s="130"/>
       <c r="G8" s="15" t="s">
         <v>532</v>
       </c>
@@ -29667,9 +29793,7 @@
       <c r="E9" s="130" t="s">
         <v>1415</v>
       </c>
-      <c r="F9" s="130" t="s">
-        <v>3</v>
-      </c>
+      <c r="F9" s="130"/>
       <c r="G9" s="15" t="s">
         <v>540</v>
       </c>
@@ -29692,9 +29816,7 @@
       <c r="E10" s="130" t="s">
         <v>1415</v>
       </c>
-      <c r="F10" s="130" t="s">
-        <v>3</v>
-      </c>
+      <c r="F10" s="130"/>
       <c r="G10" s="15" t="s">
         <v>434</v>
       </c>
@@ -29717,9 +29839,7 @@
       <c r="E11" s="130" t="s">
         <v>1415</v>
       </c>
-      <c r="F11" s="130" t="s">
-        <v>3</v>
-      </c>
+      <c r="F11" s="130"/>
       <c r="G11" s="15" t="s">
         <v>438</v>
       </c>
@@ -29740,9 +29860,7 @@
       <c r="E12" s="130" t="s">
         <v>1415</v>
       </c>
-      <c r="F12" s="130" t="s">
-        <v>3</v>
-      </c>
+      <c r="F12" s="130"/>
       <c r="G12" s="130" t="s">
         <v>3</v>
       </c>
@@ -29763,9 +29881,7 @@
       <c r="E13" s="130" t="s">
         <v>1415</v>
       </c>
-      <c r="F13" s="130" t="s">
-        <v>3</v>
-      </c>
+      <c r="F13" s="130"/>
       <c r="G13" s="15" t="s">
         <v>442</v>
       </c>
@@ -29786,9 +29902,7 @@
       <c r="E14" s="10" t="s">
         <v>1415</v>
       </c>
-      <c r="F14" s="130" t="s">
-        <v>3</v>
-      </c>
+      <c r="F14" s="130"/>
       <c r="G14" s="10" t="s">
         <v>7</v>
       </c>
@@ -29809,9 +29923,7 @@
       <c r="E15" s="10" t="s">
         <v>1415</v>
       </c>
-      <c r="F15" s="130" t="s">
-        <v>3</v>
-      </c>
+      <c r="F15" s="130"/>
       <c r="G15" s="10" t="s">
         <v>3</v>
       </c>
@@ -29832,9 +29944,7 @@
       <c r="E16" s="10" t="s">
         <v>1415</v>
       </c>
-      <c r="F16" s="130" t="s">
-        <v>3</v>
-      </c>
+      <c r="F16" s="130"/>
       <c r="G16" s="9" t="s">
         <v>3</v>
       </c>
@@ -29855,9 +29965,7 @@
       <c r="E17" s="10" t="s">
         <v>1415</v>
       </c>
-      <c r="F17" s="130" t="s">
-        <v>3</v>
-      </c>
+      <c r="F17" s="130"/>
       <c r="G17" s="10" t="s">
         <v>3</v>
       </c>
@@ -29878,9 +29986,7 @@
       <c r="E18" s="10" t="s">
         <v>1415</v>
       </c>
-      <c r="F18" s="130" t="s">
-        <v>3</v>
-      </c>
+      <c r="F18" s="130"/>
       <c r="G18" s="10" t="s">
         <v>7</v>
       </c>
@@ -29901,9 +30007,7 @@
       <c r="E19" s="10" t="s">
         <v>1415</v>
       </c>
-      <c r="F19" s="130" t="s">
-        <v>3</v>
-      </c>
+      <c r="F19" s="130"/>
       <c r="G19" s="10" t="s">
         <v>7</v>
       </c>
@@ -29924,9 +30028,7 @@
       <c r="E20" s="10" t="s">
         <v>1415</v>
       </c>
-      <c r="F20" s="130" t="s">
-        <v>3</v>
-      </c>
+      <c r="F20" s="130"/>
       <c r="G20" s="10" t="s">
         <v>3</v>
       </c>
@@ -29947,9 +30049,7 @@
       <c r="E21" s="10" t="s">
         <v>1415</v>
       </c>
-      <c r="F21" s="130" t="s">
-        <v>3</v>
-      </c>
+      <c r="F21" s="130"/>
       <c r="G21" s="10" t="s">
         <v>3</v>
       </c>
@@ -29970,9 +30070,7 @@
       <c r="E22" s="10" t="s">
         <v>1415</v>
       </c>
-      <c r="F22" s="130" t="s">
-        <v>3</v>
-      </c>
+      <c r="F22" s="130"/>
       <c r="G22" s="10" t="s">
         <v>3</v>
       </c>
@@ -29993,9 +30091,7 @@
       <c r="E23" s="10" t="s">
         <v>1415</v>
       </c>
-      <c r="F23" s="130" t="s">
-        <v>3</v>
-      </c>
+      <c r="F23" s="130"/>
       <c r="G23" s="10" t="s">
         <v>3</v>
       </c>
@@ -30016,9 +30112,7 @@
       <c r="E24" s="10" t="s">
         <v>1415</v>
       </c>
-      <c r="F24" s="130" t="s">
-        <v>3</v>
-      </c>
+      <c r="F24" s="130"/>
       <c r="G24" s="9" t="s">
         <v>7</v>
       </c>
@@ -30039,9 +30133,7 @@
       <c r="E25" s="10" t="s">
         <v>1415</v>
       </c>
-      <c r="F25" s="130" t="s">
-        <v>3</v>
-      </c>
+      <c r="F25" s="130"/>
       <c r="G25" s="9" t="s">
         <v>3</v>
       </c>
@@ -30062,9 +30154,7 @@
       <c r="E26" s="10" t="s">
         <v>1415</v>
       </c>
-      <c r="F26" s="130" t="s">
-        <v>3</v>
-      </c>
+      <c r="F26" s="130"/>
       <c r="G26" s="10" t="s">
         <v>3</v>
       </c>
@@ -30085,9 +30175,7 @@
       <c r="E27" s="10" t="s">
         <v>1415</v>
       </c>
-      <c r="F27" s="130" t="s">
-        <v>3</v>
-      </c>
+      <c r="F27" s="130"/>
       <c r="G27" s="10" t="s">
         <v>3</v>
       </c>
@@ -30108,9 +30196,7 @@
       <c r="E28" s="10" t="s">
         <v>1415</v>
       </c>
-      <c r="F28" s="130" t="s">
-        <v>3</v>
-      </c>
+      <c r="F28" s="130"/>
       <c r="G28" s="9" t="s">
         <v>7</v>
       </c>
@@ -30131,9 +30217,7 @@
       <c r="E29" s="10" t="s">
         <v>1415</v>
       </c>
-      <c r="F29" s="130" t="s">
-        <v>3</v>
-      </c>
+      <c r="F29" s="130"/>
       <c r="G29" s="9" t="s">
         <v>7</v>
       </c>
@@ -30154,9 +30238,7 @@
       <c r="E30" s="10" t="s">
         <v>1415</v>
       </c>
-      <c r="F30" s="130" t="s">
-        <v>3</v>
-      </c>
+      <c r="F30" s="130"/>
       <c r="G30" s="9" t="s">
         <v>3</v>
       </c>
@@ -30177,9 +30259,7 @@
       <c r="E31" s="10" t="s">
         <v>1415</v>
       </c>
-      <c r="F31" s="130" t="s">
-        <v>3</v>
-      </c>
+      <c r="F31" s="130"/>
       <c r="G31" s="9" t="s">
         <v>3</v>
       </c>
@@ -30200,9 +30280,7 @@
       <c r="E32" s="10" t="s">
         <v>1415</v>
       </c>
-      <c r="F32" s="130" t="s">
-        <v>3</v>
-      </c>
+      <c r="F32" s="130"/>
       <c r="G32" s="9" t="s">
         <v>3</v>
       </c>
@@ -30223,9 +30301,7 @@
       <c r="E33" s="10" t="s">
         <v>1415</v>
       </c>
-      <c r="F33" s="130" t="s">
-        <v>3</v>
-      </c>
+      <c r="F33" s="130"/>
       <c r="G33" s="9" t="s">
         <v>3</v>
       </c>
@@ -30246,9 +30322,7 @@
       <c r="E34" s="10" t="s">
         <v>1415</v>
       </c>
-      <c r="F34" s="130" t="s">
-        <v>3</v>
-      </c>
+      <c r="F34" s="130"/>
       <c r="G34" s="9" t="s">
         <v>3</v>
       </c>
@@ -30269,9 +30343,7 @@
       <c r="E35" s="10" t="s">
         <v>1415</v>
       </c>
-      <c r="F35" s="130" t="s">
-        <v>3</v>
-      </c>
+      <c r="F35" s="130"/>
       <c r="G35" s="9" t="s">
         <v>3</v>
       </c>
@@ -30292,9 +30364,7 @@
       <c r="E36" s="10" t="s">
         <v>1415</v>
       </c>
-      <c r="F36" s="130" t="s">
-        <v>3</v>
-      </c>
+      <c r="F36" s="130"/>
       <c r="G36" s="9" t="s">
         <v>7</v>
       </c>
@@ -30315,9 +30385,7 @@
       <c r="E37" s="10" t="s">
         <v>1415</v>
       </c>
-      <c r="F37" s="130" t="s">
-        <v>3</v>
-      </c>
+      <c r="F37" s="130"/>
       <c r="G37" s="9" t="s">
         <v>7</v>
       </c>
@@ -30338,9 +30406,7 @@
       <c r="E38" s="10" t="s">
         <v>1415</v>
       </c>
-      <c r="F38" s="130" t="s">
-        <v>3</v>
-      </c>
+      <c r="F38" s="130"/>
       <c r="G38" s="9" t="s">
         <v>3</v>
       </c>
@@ -30361,9 +30427,7 @@
       <c r="E39" s="10" t="s">
         <v>1415</v>
       </c>
-      <c r="F39" s="130" t="s">
-        <v>3</v>
-      </c>
+      <c r="F39" s="130"/>
       <c r="G39" s="9" t="s">
         <v>3</v>
       </c>
@@ -30384,9 +30448,7 @@
       <c r="E40" s="10" t="s">
         <v>1415</v>
       </c>
-      <c r="F40" s="130" t="s">
-        <v>3</v>
-      </c>
+      <c r="F40" s="130"/>
       <c r="G40" s="9" t="s">
         <v>3</v>
       </c>
@@ -30407,9 +30469,7 @@
       <c r="E41" s="10" t="s">
         <v>1415</v>
       </c>
-      <c r="F41" s="130" t="s">
-        <v>3</v>
-      </c>
+      <c r="F41" s="130"/>
       <c r="G41" s="9" t="s">
         <v>3</v>
       </c>
@@ -30430,9 +30490,7 @@
       <c r="E42" s="216" t="s">
         <v>1415</v>
       </c>
-      <c r="F42" s="130" t="s">
-        <v>3</v>
-      </c>
+      <c r="F42" s="130"/>
       <c r="G42" s="238" t="s">
         <v>429</v>
       </c>
@@ -30453,9 +30511,7 @@
       <c r="E43" s="216" t="s">
         <v>1415</v>
       </c>
-      <c r="F43" s="130" t="s">
-        <v>3</v>
-      </c>
+      <c r="F43" s="130"/>
       <c r="G43" s="238" t="s">
         <v>308</v>
       </c>
@@ -30476,9 +30532,7 @@
       <c r="E44" s="216" t="s">
         <v>1415</v>
       </c>
-      <c r="F44" s="130" t="s">
-        <v>3</v>
-      </c>
+      <c r="F44" s="130"/>
       <c r="G44" s="238" t="s">
         <v>262</v>
       </c>
@@ -30499,9 +30553,7 @@
       <c r="E45" s="216" t="s">
         <v>1415</v>
       </c>
-      <c r="F45" s="130" t="s">
-        <v>3</v>
-      </c>
+      <c r="F45" s="130"/>
       <c r="G45" s="238" t="s">
         <v>266</v>
       </c>
@@ -30522,9 +30574,7 @@
       <c r="E46" s="216" t="s">
         <v>1415</v>
       </c>
-      <c r="F46" s="130" t="s">
-        <v>3</v>
-      </c>
+      <c r="F46" s="130"/>
       <c r="G46" s="238" t="s">
         <v>296</v>
       </c>
@@ -30545,9 +30595,7 @@
       <c r="E47" s="216" t="s">
         <v>1415</v>
       </c>
-      <c r="F47" s="130" t="s">
-        <v>3</v>
-      </c>
+      <c r="F47" s="130"/>
       <c r="G47" s="238" t="s">
         <v>300</v>
       </c>
@@ -30568,9 +30616,7 @@
       <c r="E48" s="216" t="s">
         <v>1415</v>
       </c>
-      <c r="F48" s="130" t="s">
-        <v>3</v>
-      </c>
+      <c r="F48" s="130"/>
       <c r="G48" s="238" t="s">
         <v>132</v>
       </c>
@@ -30591,9 +30637,7 @@
       <c r="E49" s="216" t="s">
         <v>1415</v>
       </c>
-      <c r="F49" s="130" t="s">
-        <v>3</v>
-      </c>
+      <c r="F49" s="130"/>
       <c r="G49" s="238" t="s">
         <v>136</v>
       </c>
@@ -30614,9 +30658,7 @@
       <c r="E50" s="216" t="s">
         <v>1415</v>
       </c>
-      <c r="F50" s="130" t="s">
-        <v>3</v>
-      </c>
+      <c r="F50" s="130"/>
       <c r="G50" s="238" t="s">
         <v>140</v>
       </c>
@@ -30637,9 +30679,7 @@
       <c r="E51" s="216" t="s">
         <v>1415</v>
       </c>
-      <c r="F51" s="130" t="s">
-        <v>3</v>
-      </c>
+      <c r="F51" s="130"/>
       <c r="G51" s="238" t="s">
         <v>144</v>
       </c>
@@ -30660,9 +30700,7 @@
       <c r="E52" s="216" t="s">
         <v>1415</v>
       </c>
-      <c r="F52" s="130" t="s">
-        <v>3</v>
-      </c>
+      <c r="F52" s="130"/>
       <c r="G52" s="238" t="s">
         <v>148</v>
       </c>
@@ -30683,9 +30721,7 @@
       <c r="E53" s="216" t="s">
         <v>1415</v>
       </c>
-      <c r="F53" s="130" t="s">
-        <v>3</v>
-      </c>
+      <c r="F53" s="130"/>
       <c r="G53" s="15" t="s">
         <v>152</v>
       </c>
@@ -30706,9 +30742,7 @@
       <c r="E54" s="130" t="s">
         <v>1415</v>
       </c>
-      <c r="F54" s="130" t="s">
-        <v>3</v>
-      </c>
+      <c r="F54" s="130"/>
       <c r="G54" s="130" t="s">
         <v>7</v>
       </c>
@@ -30729,9 +30763,7 @@
       <c r="E55" s="130" t="s">
         <v>1415</v>
       </c>
-      <c r="F55" s="130" t="s">
-        <v>3</v>
-      </c>
+      <c r="F55" s="130"/>
       <c r="G55" s="216" t="s">
         <v>7</v>
       </c>
@@ -30752,9 +30784,7 @@
       <c r="E56" s="130" t="s">
         <v>1415</v>
       </c>
-      <c r="F56" s="130" t="s">
-        <v>3</v>
-      </c>
+      <c r="F56" s="130"/>
       <c r="G56" s="15" t="s">
         <v>156</v>
       </c>
@@ -30775,9 +30805,7 @@
       <c r="E57" s="130" t="s">
         <v>1415</v>
       </c>
-      <c r="F57" s="130" t="s">
-        <v>3</v>
-      </c>
+      <c r="F57" s="130"/>
       <c r="G57" s="238" t="s">
         <v>160</v>
       </c>
@@ -30798,9 +30826,7 @@
       <c r="E58" s="130" t="s">
         <v>1415</v>
       </c>
-      <c r="F58" s="130" t="s">
-        <v>3</v>
-      </c>
+      <c r="F58" s="130"/>
       <c r="G58" s="15" t="s">
         <v>164</v>
       </c>
@@ -30821,9 +30847,7 @@
       <c r="E59" s="130" t="s">
         <v>1415</v>
       </c>
-      <c r="F59" s="130" t="s">
-        <v>3</v>
-      </c>
+      <c r="F59" s="130"/>
       <c r="G59" s="15" t="s">
         <v>204</v>
       </c>
@@ -30845,9 +30869,7 @@
       <c r="E60" s="130" t="s">
         <v>1415</v>
       </c>
-      <c r="F60" s="130" t="s">
-        <v>3</v>
-      </c>
+      <c r="F60" s="130"/>
       <c r="G60" s="15" t="s">
         <v>208</v>
       </c>
@@ -30868,9 +30890,7 @@
       <c r="E61" s="130" t="s">
         <v>1415</v>
       </c>
-      <c r="F61" s="130" t="s">
-        <v>3</v>
-      </c>
+      <c r="F61" s="130"/>
       <c r="G61" s="15" t="s">
         <v>212</v>
       </c>
@@ -30891,9 +30911,7 @@
       <c r="E62" s="130" t="s">
         <v>1415</v>
       </c>
-      <c r="F62" s="130" t="s">
-        <v>3</v>
-      </c>
+      <c r="F62" s="130"/>
       <c r="G62" s="15" t="s">
         <v>216</v>
       </c>
@@ -30914,9 +30932,7 @@
       <c r="E63" s="130" t="s">
         <v>1415</v>
       </c>
-      <c r="F63" s="130" t="s">
-        <v>3</v>
-      </c>
+      <c r="F63" s="130"/>
       <c r="G63" s="15" t="s">
         <v>413</v>
       </c>
@@ -30937,9 +30953,7 @@
       <c r="E64" s="130" t="s">
         <v>1415</v>
       </c>
-      <c r="F64" s="130" t="s">
-        <v>3</v>
-      </c>
+      <c r="F64" s="130"/>
       <c r="G64" s="15" t="s">
         <v>312</v>
       </c>
@@ -30960,9 +30974,7 @@
       <c r="E65" s="130" t="s">
         <v>1415</v>
       </c>
-      <c r="F65" s="130" t="s">
-        <v>3</v>
-      </c>
+      <c r="F65" s="130"/>
       <c r="G65" s="15" t="s">
         <v>316</v>
       </c>
@@ -30983,9 +30995,7 @@
       <c r="E66" s="130" t="s">
         <v>1415</v>
       </c>
-      <c r="F66" s="130" t="s">
-        <v>3</v>
-      </c>
+      <c r="F66" s="130"/>
       <c r="G66" s="15" t="s">
         <v>339</v>
       </c>
@@ -31006,9 +31016,7 @@
       <c r="E67" s="130" t="s">
         <v>1415</v>
       </c>
-      <c r="F67" s="130" t="s">
-        <v>3</v>
-      </c>
+      <c r="F67" s="130"/>
       <c r="G67" s="15" t="s">
         <v>347</v>
       </c>
@@ -31029,9 +31037,7 @@
       <c r="E68" s="130" t="s">
         <v>1415</v>
       </c>
-      <c r="F68" s="130" t="s">
-        <v>3</v>
-      </c>
+      <c r="F68" s="130"/>
       <c r="G68" s="15" t="s">
         <v>351</v>
       </c>
@@ -31052,9 +31058,7 @@
       <c r="E69" s="130" t="s">
         <v>1415</v>
       </c>
-      <c r="F69" s="130" t="s">
-        <v>3</v>
-      </c>
+      <c r="F69" s="130"/>
       <c r="G69" s="15" t="s">
         <v>355</v>
       </c>
@@ -31075,9 +31079,7 @@
       <c r="E70" s="130" t="s">
         <v>1415</v>
       </c>
-      <c r="F70" s="130" t="s">
-        <v>3</v>
-      </c>
+      <c r="F70" s="130"/>
       <c r="G70" s="15" t="s">
         <v>359</v>
       </c>
@@ -31098,9 +31100,7 @@
       <c r="E71" s="130" t="s">
         <v>1415</v>
       </c>
-      <c r="F71" s="130" t="s">
-        <v>3</v>
-      </c>
+      <c r="F71" s="130"/>
       <c r="G71" s="15" t="s">
         <v>367</v>
       </c>
@@ -31121,9 +31121,7 @@
       <c r="E72" s="130" t="s">
         <v>1415</v>
       </c>
-      <c r="F72" s="130" t="s">
-        <v>3</v>
-      </c>
+      <c r="F72" s="130"/>
       <c r="G72" s="15" t="s">
         <v>250</v>
       </c>
@@ -31144,9 +31142,7 @@
       <c r="E73" s="130" t="s">
         <v>1415</v>
       </c>
-      <c r="F73" s="130" t="s">
-        <v>3</v>
-      </c>
+      <c r="F73" s="130"/>
       <c r="G73" s="15" t="s">
         <v>254</v>
       </c>
@@ -31167,9 +31163,7 @@
       <c r="E74" s="130" t="s">
         <v>1415</v>
       </c>
-      <c r="F74" s="130" t="s">
-        <v>3</v>
-      </c>
+      <c r="F74" s="130"/>
       <c r="G74" s="15" t="s">
         <v>258</v>
       </c>
@@ -31190,9 +31184,7 @@
       <c r="E75" s="130" t="s">
         <v>1415</v>
       </c>
-      <c r="F75" s="130" t="s">
-        <v>3</v>
-      </c>
+      <c r="F75" s="130"/>
       <c r="G75" s="15" t="s">
         <v>279</v>
       </c>
@@ -31213,9 +31205,7 @@
       <c r="E76" s="130" t="s">
         <v>1415</v>
       </c>
-      <c r="F76" s="130" t="s">
-        <v>3</v>
-      </c>
+      <c r="F76" s="130"/>
       <c r="G76" s="15" t="s">
         <v>220</v>
       </c>
@@ -31236,9 +31226,7 @@
       <c r="E77" s="130" t="s">
         <v>1415</v>
       </c>
-      <c r="F77" s="130" t="s">
-        <v>3</v>
-      </c>
+      <c r="F77" s="130"/>
       <c r="G77" s="15" t="s">
         <v>224</v>
       </c>
@@ -31261,9 +31249,7 @@
       <c r="E78" s="130" t="s">
         <v>1415</v>
       </c>
-      <c r="F78" s="130" t="s">
-        <v>3</v>
-      </c>
+      <c r="F78" s="130"/>
       <c r="G78" s="15" t="s">
         <v>172</v>
       </c>
@@ -31285,9 +31271,7 @@
       <c r="E79" s="130" t="s">
         <v>1415</v>
       </c>
-      <c r="F79" s="130" t="s">
-        <v>3</v>
-      </c>
+      <c r="F79" s="130"/>
       <c r="G79" s="15" t="s">
         <v>111</v>
       </c>
@@ -31308,9 +31292,7 @@
       <c r="E80" s="130" t="s">
         <v>1415</v>
       </c>
-      <c r="F80" s="130" t="s">
-        <v>3</v>
-      </c>
+      <c r="F80" s="130"/>
       <c r="G80" s="15" t="s">
         <v>115</v>
       </c>
@@ -31331,9 +31313,7 @@
       <c r="E81" s="130" t="s">
         <v>1415</v>
       </c>
-      <c r="F81" s="130" t="s">
-        <v>3</v>
-      </c>
+      <c r="F81" s="130"/>
       <c r="G81" s="15" t="s">
         <v>343</v>
       </c>
@@ -31356,9 +31336,7 @@
       <c r="E82" s="130" t="s">
         <v>1415</v>
       </c>
-      <c r="F82" s="130" t="s">
-        <v>3</v>
-      </c>
+      <c r="F82" s="130"/>
       <c r="G82" s="130" t="s">
         <v>3</v>
       </c>
@@ -31379,9 +31357,7 @@
       <c r="E83" s="130" t="s">
         <v>1415</v>
       </c>
-      <c r="F83" s="130" t="s">
-        <v>3</v>
-      </c>
+      <c r="F83" s="130"/>
       <c r="G83" s="15" t="s">
         <v>272</v>
       </c>
@@ -31404,9 +31380,7 @@
       <c r="E84" s="130" t="s">
         <v>1415</v>
       </c>
-      <c r="F84" s="130" t="s">
-        <v>3</v>
-      </c>
+      <c r="F84" s="130"/>
       <c r="G84" s="15" t="s">
         <v>450</v>
       </c>
@@ -31429,9 +31403,7 @@
       <c r="E85" s="130" t="s">
         <v>1415</v>
       </c>
-      <c r="F85" s="130" t="s">
-        <v>3</v>
-      </c>
+      <c r="F85" s="130"/>
       <c r="G85" s="15" t="s">
         <v>417</v>
       </c>
@@ -31452,9 +31424,7 @@
       <c r="E86" s="130" t="s">
         <v>1415</v>
       </c>
-      <c r="F86" s="130" t="s">
-        <v>3</v>
-      </c>
+      <c r="F86" s="130"/>
       <c r="G86" s="15" t="s">
         <v>432</v>
       </c>
@@ -31475,9 +31445,7 @@
       <c r="E87" s="130" t="s">
         <v>1415</v>
       </c>
-      <c r="F87" s="130" t="s">
-        <v>3</v>
-      </c>
+      <c r="F87" s="130"/>
       <c r="G87" s="15" t="s">
         <v>335</v>
       </c>
@@ -32192,7 +32160,9 @@
       <c r="E118" s="130" t="s">
         <v>1412</v>
       </c>
-      <c r="F118" s="130"/>
+      <c r="F118" s="130" t="s">
+        <v>3</v>
+      </c>
       <c r="G118" s="15" t="s">
         <v>286</v>
       </c>
@@ -32694,7 +32664,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="140" spans="1:9" ht="12"/>
+    <row r="140" spans="1:9" ht="12">
+      <c r="F140" s="270" t="s">
+        <v>1493</v>
+      </c>
+    </row>
     <row r="141" spans="1:9" ht="12">
       <c r="C141" s="122" t="s">
         <v>1480</v>
@@ -32703,6 +32677,13 @@
         <f>COUNTIF(D5:D139,"y")</f>
         <v>52</v>
       </c>
+      <c r="E141" s="164" t="s">
+        <v>1499</v>
+      </c>
+      <c r="F141" s="164">
+        <f>COUNTIF(F5:F139,"n")</f>
+        <v>8</v>
+      </c>
     </row>
     <row r="142" spans="1:9" ht="12">
       <c r="C142" s="9" t="s">
@@ -32710,6 +32691,13 @@
       </c>
       <c r="D142" s="9">
         <f>COUNTIF(E88:E139,"TP")</f>
+        <v>52</v>
+      </c>
+      <c r="E142" s="168" t="s">
+        <v>1500</v>
+      </c>
+      <c r="F142" s="164">
+        <f>COUNTA(F5:F139)</f>
         <v>52</v>
       </c>
     </row>
@@ -33687,8 +33675,8 @@
   <dimension ref="A1:J62"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:A1048576"/>
+      <pane ySplit="3" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -35319,9 +35307,9 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:U927"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A10" sqref="A10:B10"/>
+      <selection pane="bottomLeft" activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -35422,11 +35410,11 @@
       </c>
       <c r="E3" s="128">
         <f>COUNTIF(E4:E102,"TP")/COUNTA(E4:E102)</f>
-        <v>0.77777777777777779</v>
+        <v>0.76767676767676762</v>
       </c>
       <c r="F3" s="211">
         <f>COUNTIF(F4:F102,"y")</f>
-        <v>98</v>
+        <v>77</v>
       </c>
       <c r="G3" s="128">
         <f>COUNTIF(G4:G102,"NC")/COUNTA(G4:G102)</f>
@@ -35454,9 +35442,7 @@
       <c r="E4" s="130" t="s">
         <v>1418</v>
       </c>
-      <c r="F4" s="130" t="s">
-        <v>3</v>
-      </c>
+      <c r="F4" s="130"/>
       <c r="G4" s="130" t="s">
         <v>1416</v>
       </c>
@@ -35473,7 +35459,7 @@
       <c r="B5" s="79" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="259" t="s">
+      <c r="C5" s="254" t="s">
         <v>1420</v>
       </c>
       <c r="D5" s="130" t="s">
@@ -35482,9 +35468,7 @@
       <c r="E5" s="130" t="s">
         <v>1415</v>
       </c>
-      <c r="F5" s="130" t="s">
-        <v>3</v>
-      </c>
+      <c r="F5" s="130"/>
       <c r="G5" s="130" t="s">
         <v>1416</v>
       </c>
@@ -35512,9 +35496,7 @@
       <c r="E6" s="130" t="s">
         <v>1415</v>
       </c>
-      <c r="F6" s="130" t="s">
-        <v>3</v>
-      </c>
+      <c r="F6" s="130"/>
       <c r="G6" s="130" t="s">
         <v>1416</v>
       </c>
@@ -35542,9 +35524,7 @@
       <c r="E7" s="130" t="s">
         <v>1415</v>
       </c>
-      <c r="F7" s="130" t="s">
-        <v>3</v>
-      </c>
+      <c r="F7" s="130"/>
       <c r="G7" s="130" t="s">
         <v>1416</v>
       </c>
@@ -35572,9 +35552,7 @@
       <c r="E8" s="130" t="s">
         <v>1415</v>
       </c>
-      <c r="F8" s="130" t="s">
-        <v>3</v>
-      </c>
+      <c r="F8" s="130"/>
       <c r="G8" s="130" t="s">
         <v>1416</v>
       </c>
@@ -35599,9 +35577,7 @@
       <c r="E9" s="130" t="s">
         <v>1415</v>
       </c>
-      <c r="F9" s="130" t="s">
-        <v>3</v>
-      </c>
+      <c r="F9" s="130"/>
       <c r="G9" s="130" t="s">
         <v>1416</v>
       </c>
@@ -35629,9 +35605,7 @@
       <c r="E10" s="130" t="s">
         <v>1415</v>
       </c>
-      <c r="F10" s="130" t="s">
-        <v>3</v>
-      </c>
+      <c r="F10" s="130"/>
       <c r="G10" s="130" t="s">
         <v>1416</v>
       </c>
@@ -35659,9 +35633,7 @@
       <c r="E11" s="130" t="s">
         <v>1415</v>
       </c>
-      <c r="F11" s="130" t="s">
-        <v>3</v>
-      </c>
+      <c r="F11" s="130"/>
       <c r="G11" s="130" t="s">
         <v>1416</v>
       </c>
@@ -35685,9 +35657,7 @@
       <c r="E12" s="130" t="s">
         <v>1415</v>
       </c>
-      <c r="F12" s="130" t="s">
-        <v>3</v>
-      </c>
+      <c r="F12" s="130"/>
       <c r="G12" s="130" t="s">
         <v>1416</v>
       </c>
@@ -35713,11 +35683,9 @@
         <v>7</v>
       </c>
       <c r="E13" s="130" t="s">
-        <v>1412</v>
-      </c>
-      <c r="F13" s="130" t="s">
-        <v>3</v>
-      </c>
+        <v>1415</v>
+      </c>
+      <c r="F13" s="130"/>
       <c r="G13" s="130" t="s">
         <v>1416</v>
       </c>
@@ -35741,9 +35709,7 @@
       <c r="E14" s="130" t="s">
         <v>1415</v>
       </c>
-      <c r="F14" s="130" t="s">
-        <v>3</v>
-      </c>
+      <c r="F14" s="130"/>
       <c r="G14" s="130" t="s">
         <v>1416</v>
       </c>
@@ -35767,9 +35733,7 @@
       <c r="E15" s="130" t="s">
         <v>1415</v>
       </c>
-      <c r="F15" s="130" t="s">
-        <v>3</v>
-      </c>
+      <c r="F15" s="130"/>
       <c r="G15" s="130" t="s">
         <v>1416</v>
       </c>
@@ -35793,9 +35757,7 @@
       <c r="E16" s="130" t="s">
         <v>1415</v>
       </c>
-      <c r="F16" s="130" t="s">
-        <v>3</v>
-      </c>
+      <c r="F16" s="130"/>
       <c r="G16" s="130" t="s">
         <v>1416</v>
       </c>
@@ -35823,9 +35785,7 @@
       <c r="E17" s="130" t="s">
         <v>1415</v>
       </c>
-      <c r="F17" s="130" t="s">
-        <v>3</v>
-      </c>
+      <c r="F17" s="130"/>
       <c r="G17" s="130" t="s">
         <v>1416</v>
       </c>
@@ -35840,7 +35800,7 @@
       <c r="B18" s="83" t="s">
         <v>2</v>
       </c>
-      <c r="C18" s="260" t="s">
+      <c r="C18" s="255" t="s">
         <v>1425</v>
       </c>
       <c r="D18" s="130" t="s">
@@ -35849,9 +35809,7 @@
       <c r="E18" s="130" t="s">
         <v>1415</v>
       </c>
-      <c r="F18" s="130" t="s">
-        <v>3</v>
-      </c>
+      <c r="F18" s="130"/>
       <c r="G18" s="130" t="s">
         <v>1416</v>
       </c>
@@ -35866,7 +35824,7 @@
       <c r="B19" s="83" t="s">
         <v>2</v>
       </c>
-      <c r="C19" s="260" t="s">
+      <c r="C19" s="255" t="s">
         <v>1426</v>
       </c>
       <c r="D19" s="130" t="s">
@@ -35875,9 +35833,7 @@
       <c r="E19" s="130" t="s">
         <v>1415</v>
       </c>
-      <c r="F19" s="130" t="s">
-        <v>3</v>
-      </c>
+      <c r="F19" s="130"/>
       <c r="G19" s="130" t="s">
         <v>1416</v>
       </c>
@@ -35901,9 +35857,7 @@
       <c r="E20" s="130" t="s">
         <v>1415</v>
       </c>
-      <c r="F20" s="130" t="s">
-        <v>3</v>
-      </c>
+      <c r="F20" s="130"/>
       <c r="G20" s="130" t="s">
         <v>1416</v>
       </c>
@@ -35927,9 +35881,7 @@
       <c r="E21" s="130" t="s">
         <v>1415</v>
       </c>
-      <c r="F21" s="130" t="s">
-        <v>3</v>
-      </c>
+      <c r="F21" s="130"/>
       <c r="G21" s="130" t="s">
         <v>1416</v>
       </c>
@@ -35957,9 +35909,7 @@
       <c r="E22" s="130" t="s">
         <v>1415</v>
       </c>
-      <c r="F22" s="130" t="s">
-        <v>3</v>
-      </c>
+      <c r="F22" s="130"/>
       <c r="G22" s="130" t="s">
         <v>1416</v>
       </c>
@@ -35977,19 +35927,17 @@
       <c r="C23" s="83" t="s">
         <v>6</v>
       </c>
-      <c r="D23" s="261" t="s">
-        <v>7</v>
-      </c>
-      <c r="E23" s="262" t="s">
+      <c r="D23" s="256" t="s">
+        <v>7</v>
+      </c>
+      <c r="E23" s="257" t="s">
         <v>1415</v>
       </c>
-      <c r="F23" s="130" t="s">
-        <v>3</v>
-      </c>
-      <c r="G23" s="262" t="s">
+      <c r="F23" s="130"/>
+      <c r="G23" s="257" t="s">
         <v>1416</v>
       </c>
-      <c r="H23" s="261" t="s">
+      <c r="H23" s="256" t="s">
         <v>3</v>
       </c>
       <c r="L23" s="238"/>
@@ -36010,9 +35958,7 @@
       <c r="E24" s="130" t="s">
         <v>1415</v>
       </c>
-      <c r="F24" s="130" t="s">
-        <v>3</v>
-      </c>
+      <c r="F24" s="130"/>
       <c r="G24" s="130" t="s">
         <v>1416</v>
       </c>
@@ -36034,7 +35980,7 @@
       </c>
     </row>
     <row r="25" spans="1:12" s="9" customFormat="1" ht="22">
-      <c r="A25" s="263">
+      <c r="A25" s="258">
         <v>25161820</v>
       </c>
       <c r="B25" s="79" t="s">
@@ -36064,7 +36010,7 @@
       <c r="L25" s="12"/>
     </row>
     <row r="26" spans="1:12" s="9" customFormat="1" ht="22">
-      <c r="A26" s="263">
+      <c r="A26" s="258">
         <v>25161820</v>
       </c>
       <c r="B26" s="79" t="s">
@@ -36088,19 +36034,19 @@
       <c r="H26" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="I26" s="264"/>
-      <c r="J26" s="264"/>
-      <c r="K26" s="264"/>
+      <c r="I26" s="259"/>
+      <c r="J26" s="259"/>
+      <c r="K26" s="259"/>
       <c r="L26" s="12"/>
     </row>
     <row r="27" spans="1:12" s="9" customFormat="1" ht="39">
-      <c r="A27" s="263">
+      <c r="A27" s="258">
         <v>25161820</v>
       </c>
       <c r="B27" s="79" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="265" t="s">
+      <c r="C27" s="260" t="s">
         <v>1417</v>
       </c>
       <c r="D27" s="130" t="s">
@@ -36118,13 +36064,13 @@
       <c r="H27" s="130" t="s">
         <v>3</v>
       </c>
-      <c r="I27" s="264"/>
-      <c r="J27" s="264"/>
-      <c r="K27" s="264"/>
+      <c r="I27" s="259"/>
+      <c r="J27" s="259"/>
+      <c r="K27" s="259"/>
       <c r="L27" s="12"/>
     </row>
     <row r="28" spans="1:12" s="9" customFormat="1" ht="24">
-      <c r="A28" s="263">
+      <c r="A28" s="258">
         <v>25328847</v>
       </c>
       <c r="B28" s="83" t="s">
@@ -36553,7 +36499,7 @@
       <c r="B42" s="79" t="s">
         <v>25</v>
       </c>
-      <c r="C42" s="266" t="s">
+      <c r="C42" s="261" t="s">
         <v>93</v>
       </c>
       <c r="D42" s="15" t="s">
@@ -37091,7 +37037,7 @@
       <c r="B61" s="79" t="s">
         <v>2</v>
       </c>
-      <c r="C61" s="260" t="s">
+      <c r="C61" s="255" t="s">
         <v>1429</v>
       </c>
       <c r="D61" s="130" t="s">
@@ -37708,19 +37654,19 @@
       <c r="C84" s="83" t="s">
         <v>5</v>
       </c>
-      <c r="D84" s="261" t="s">
-        <v>3</v>
-      </c>
-      <c r="E84" s="262" t="s">
+      <c r="D84" s="256" t="s">
+        <v>3</v>
+      </c>
+      <c r="E84" s="257" t="s">
         <v>1412</v>
       </c>
       <c r="F84" s="130" t="s">
         <v>3</v>
       </c>
-      <c r="G84" s="262" t="s">
+      <c r="G84" s="257" t="s">
         <v>1416</v>
       </c>
-      <c r="H84" s="261" t="s">
+      <c r="H84" s="256" t="s">
         <v>3</v>
       </c>
       <c r="I84" s="12"/>
@@ -38220,6 +38166,10 @@
     </row>
     <row r="103" spans="1:12" ht="15.75" customHeight="1">
       <c r="C103" s="3"/>
+      <c r="E103" s="9"/>
+      <c r="F103" s="270" t="s">
+        <v>1493</v>
+      </c>
     </row>
     <row r="104" spans="1:12" ht="15.75" customHeight="1">
       <c r="C104" s="121" t="s">
@@ -38229,6 +38179,13 @@
         <f>COUNTIF(D25:D102,"y")</f>
         <v>78</v>
       </c>
+      <c r="E104" s="164" t="s">
+        <v>1499</v>
+      </c>
+      <c r="F104" s="271">
+        <f>COUNTIF(F4:F102,"n")</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="105" spans="1:12" ht="15.75" customHeight="1">
       <c r="C105" t="s">
@@ -38238,6 +38195,13 @@
         <f>COUNTIF(E25:E102,"TP")</f>
         <v>76</v>
       </c>
+      <c r="E105" s="168" t="s">
+        <v>1500</v>
+      </c>
+      <c r="F105" s="271">
+        <f>COUNTA(F4:F102)</f>
+        <v>78</v>
+      </c>
     </row>
     <row r="106" spans="1:12" ht="15.75" customHeight="1">
       <c r="C106" t="s">
@@ -38287,7 +38251,7 @@
       </c>
       <c r="D112">
         <f>COUNTIF(E4:E102,"TP")</f>
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="113" spans="3:4" ht="15.75" customHeight="1">
@@ -38314,7 +38278,7 @@
       </c>
       <c r="D115">
         <f>COUNTIF(E4:E102,"FN")</f>
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="116" spans="3:4" ht="15.75" customHeight="1">
@@ -40774,7 +40738,7 @@
   <dimension ref="A2:G28"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -40901,7 +40865,7 @@
       </c>
       <c r="C9">
         <f>'Software- POST C v NC'!D112</f>
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D9">
         <f>'Software- POST C v NC'!D113</f>
@@ -40913,11 +40877,11 @@
       </c>
       <c r="F9">
         <f>'Software- POST C v NC'!D115</f>
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G9" s="208">
         <f>(C9)/(C9+F9)</f>
-        <v>0.80208333333333337</v>
+        <v>0.79166666666666663</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -41038,7 +41002,7 @@
       </c>
       <c r="C17">
         <f t="shared" ref="C17:F17" si="1">C9</f>
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D17">
         <f t="shared" si="1"/>
@@ -41050,11 +41014,11 @@
       </c>
       <c r="F17">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G17" s="208">
         <f>(C17)/(C17+E17)</f>
-        <v>0.96250000000000002</v>
+        <v>0.96202531645569622</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -41085,15 +41049,15 @@
       </c>
       <c r="B21" s="212">
         <f>'Antibody-POST 1st vs 2nd Abs'!F3</f>
-        <v>415</v>
+        <v>379</v>
       </c>
       <c r="C21">
-        <f>'Antibody-POST 1st vs 2nd Abs'!D465</f>
-        <v>452</v>
+        <f>'Antibody-POST 1st vs 2nd Abs'!F459</f>
+        <v>416</v>
       </c>
       <c r="D21" s="156">
         <f>B21/C21</f>
-        <v>0.91814159292035402</v>
+        <v>0.91105769230769229</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -41102,15 +41066,15 @@
       </c>
       <c r="B22" s="212">
         <f>'Organisms- POST'!F4</f>
-        <v>126</v>
+        <v>44</v>
       </c>
       <c r="C22">
-        <f>'Organisms- POST'!D148</f>
-        <v>135</v>
+        <f>'Organisms- POST'!F142</f>
+        <v>52</v>
       </c>
       <c r="D22" s="156">
         <f>B22/C22</f>
-        <v>0.93333333333333335</v>
+        <v>0.84615384615384615</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -41119,25 +41083,25 @@
       </c>
       <c r="B23" s="212">
         <f>'Software- POST C v NC'!F3</f>
-        <v>98</v>
+        <v>77</v>
       </c>
       <c r="C23">
-        <f>'Software- POST C v NC'!D111</f>
-        <v>99</v>
+        <f>'Software- POST C v NC'!F105</f>
+        <v>78</v>
       </c>
       <c r="D23" s="156">
         <f>B23/C23</f>
-        <v>0.98989898989898994</v>
+        <v>0.98717948717948723</v>
       </c>
     </row>
     <row r="25" spans="1:7">
-      <c r="B25" t="s">
+      <c r="B25" s="41" t="s">
         <v>1495</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="41" t="s">
         <v>1370</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D25" s="41" t="s">
         <v>1</v>
       </c>
     </row>
@@ -41155,7 +41119,7 @@
       </c>
       <c r="D26" s="217">
         <f>G9</f>
-        <v>0.80208333333333337</v>
+        <v>0.79166666666666663</v>
       </c>
     </row>
     <row r="27" spans="1:7">
@@ -41172,7 +41136,7 @@
       </c>
       <c r="D27" s="217">
         <f>G17</f>
-        <v>0.96250000000000002</v>
+        <v>0.96202531645569622</v>
       </c>
     </row>
     <row r="28" spans="1:7">
@@ -41181,15 +41145,15 @@
       </c>
       <c r="B28" s="217">
         <f>D21</f>
-        <v>0.91814159292035402</v>
+        <v>0.91105769230769229</v>
       </c>
       <c r="C28" s="217">
         <f>D22</f>
-        <v>0.93333333333333335</v>
+        <v>0.84615384615384615</v>
       </c>
       <c r="D28" s="217">
         <f>D23</f>
-        <v>0.98989898989898994</v>
+        <v>0.98717948717948723</v>
       </c>
     </row>
   </sheetData>
@@ -41208,8 +41172,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView topLeftCell="A4" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -41262,7 +41226,7 @@
       </c>
       <c r="B4" s="95">
         <f>B8</f>
-        <v>0.95871559633027525</v>
+        <v>0.96017699115044253</v>
       </c>
       <c r="C4" s="95">
         <f>B11</f>
@@ -41314,15 +41278,15 @@
       </c>
       <c r="B8" s="103">
         <f>D8/C8</f>
-        <v>0.95871559633027525</v>
+        <v>0.96017699115044253</v>
       </c>
       <c r="C8" s="101">
         <f>'Antibody-POST 1st vs 2nd Abs'!K2</f>
-        <v>436</v>
+        <v>452</v>
       </c>
       <c r="D8" s="101">
         <f>'Antibody-POST 1st vs 2nd Abs'!J2</f>
-        <v>418</v>
+        <v>434</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="15">
@@ -41463,21 +41427,21 @@
       </c>
       <c r="B18" s="113">
         <f>B8</f>
-        <v>0.95871559633027525</v>
+        <v>0.96017699115044253</v>
       </c>
       <c r="C18" s="32">
-        <v>0.97535000000000005</v>
+        <v>0.97623000000000004</v>
       </c>
       <c r="D18" s="32">
-        <v>0.93554000000000004</v>
+        <v>0.93779000000000001</v>
       </c>
       <c r="E18" s="22">
         <f>ABS(B18-D18)</f>
-        <v>2.3175596330275217E-2</v>
+        <v>2.2386991150442515E-2</v>
       </c>
       <c r="F18" s="23">
         <f>ABS(B18-C18)</f>
-        <v>1.6634403669724795E-2</v>
+        <v>1.6053008849557515E-2</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -41613,16 +41577,16 @@
     </row>
     <row r="26" spans="1:6" s="9" customFormat="1"/>
     <row r="27" spans="1:6">
-      <c r="A27" s="254" t="s">
+      <c r="A27" s="264" t="s">
         <v>981</v>
       </c>
-      <c r="B27" s="254"/>
-      <c r="C27" s="254"/>
-      <c r="D27" s="255" t="s">
+      <c r="B27" s="264"/>
+      <c r="C27" s="264"/>
+      <c r="D27" s="265" t="s">
         <v>982</v>
       </c>
-      <c r="E27" s="256"/>
-      <c r="F27" s="256"/>
+      <c r="E27" s="266"/>
+      <c r="F27" s="266"/>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" s="18" t="s">
@@ -41661,11 +41625,11 @@
       </c>
       <c r="E29" s="27">
         <f>E18</f>
-        <v>2.3175596330275217E-2</v>
+        <v>2.2386991150442515E-2</v>
       </c>
       <c r="F29" s="31">
         <f>F18</f>
-        <v>1.6634403669724795E-2</v>
+        <v>1.6053008849557515E-2</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -41823,23 +41787,23 @@
     </row>
     <row r="4" spans="2:13" ht="15">
       <c r="B4" s="44"/>
-      <c r="C4" s="257" t="s">
+      <c r="C4" s="267" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="257"/>
-      <c r="E4" s="257"/>
-      <c r="F4" s="257" t="s">
+      <c r="D4" s="267"/>
+      <c r="E4" s="267"/>
+      <c r="F4" s="267" t="s">
         <v>1370</v>
       </c>
-      <c r="G4" s="257"/>
-      <c r="H4" s="257"/>
-      <c r="I4" s="257"/>
-      <c r="J4" s="257" t="s">
+      <c r="G4" s="267"/>
+      <c r="H4" s="267"/>
+      <c r="I4" s="267"/>
+      <c r="J4" s="267" t="s">
         <v>1</v>
       </c>
-      <c r="K4" s="257"/>
-      <c r="L4" s="257"/>
-      <c r="M4" s="257"/>
+      <c r="K4" s="267"/>
+      <c r="L4" s="267"/>
+      <c r="M4" s="267"/>
     </row>
     <row r="5" spans="2:13" ht="16">
       <c r="C5" s="42" t="s">
@@ -42038,41 +42002,41 @@
       </c>
     </row>
     <row r="14" spans="2:13">
-      <c r="C14" s="258" t="s">
+      <c r="C14" s="268" t="s">
         <v>1365</v>
       </c>
-      <c r="D14" s="258"/>
-      <c r="E14" s="258"/>
-      <c r="F14" s="258"/>
-      <c r="G14" s="258"/>
+      <c r="D14" s="268"/>
+      <c r="E14" s="268"/>
+      <c r="F14" s="268"/>
+      <c r="G14" s="268"/>
     </row>
     <row r="15" spans="2:13">
-      <c r="C15" s="258"/>
-      <c r="D15" s="258"/>
-      <c r="E15" s="258"/>
-      <c r="F15" s="258"/>
-      <c r="G15" s="258"/>
+      <c r="C15" s="268"/>
+      <c r="D15" s="268"/>
+      <c r="E15" s="268"/>
+      <c r="F15" s="268"/>
+      <c r="G15" s="268"/>
     </row>
     <row r="16" spans="2:13">
-      <c r="C16" s="258"/>
-      <c r="D16" s="258"/>
-      <c r="E16" s="258"/>
-      <c r="F16" s="258"/>
-      <c r="G16" s="258"/>
+      <c r="C16" s="268"/>
+      <c r="D16" s="268"/>
+      <c r="E16" s="268"/>
+      <c r="F16" s="268"/>
+      <c r="G16" s="268"/>
     </row>
     <row r="17" spans="3:7">
-      <c r="C17" s="258"/>
-      <c r="D17" s="258"/>
-      <c r="E17" s="258"/>
-      <c r="F17" s="258"/>
-      <c r="G17" s="258"/>
+      <c r="C17" s="268"/>
+      <c r="D17" s="268"/>
+      <c r="E17" s="268"/>
+      <c r="F17" s="268"/>
+      <c r="G17" s="268"/>
     </row>
     <row r="18" spans="3:7">
-      <c r="C18" s="258"/>
-      <c r="D18" s="258"/>
-      <c r="E18" s="258"/>
-      <c r="F18" s="258"/>
-      <c r="G18" s="258"/>
+      <c r="C18" s="268"/>
+      <c r="D18" s="268"/>
+      <c r="E18" s="268"/>
+      <c r="F18" s="268"/>
+      <c r="G18" s="268"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>